<commit_message>
Got the matrix working, but I need more data points
</commit_message>
<xml_diff>
--- a/MatchAnalysis/DataFiles/SampleMatches.xlsx
+++ b/MatchAnalysis/DataFiles/SampleMatches.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\may_884771\Desktop\GitHub\ScoutingAnalyzer\MatchColor\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\may_884771\Desktop\GitHub\ScoutingAnalyzer\MatchAnalysis\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -10361,7 +10361,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection sqref="A1:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10535,7 +10535,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7">
-        <v>55890</v>
+        <v>5890</v>
       </c>
       <c r="C9" s="7">
         <v>4291</v>

</xml_diff>